<commit_message>
Change Maximize to FullScreen
</commit_message>
<xml_diff>
--- a/src/test/resources/Excel/CloudPos.xlsx
+++ b/src/test/resources/Excel/CloudPos.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\DenovoPortal Automation Monitoring System\src\test\resources\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF141EA3-F33D-4E89-8BF8-A10A8202164C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17179F97-3287-4B80-ADA8-0DCBA3274362}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="1" activeTab="2" xr2:uid="{411B86E3-5BC8-4162-9D5B-60D77C5E31A0}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" firstSheet="1" activeTab="2" xr2:uid="{411B86E3-5BC8-4162-9D5B-60D77C5E31A0}"/>
   </bookViews>
   <sheets>
     <sheet name="Quick Sale" sheetId="1" r:id="rId1"/>

</xml_diff>